<commit_message>
hours update CFP update
</commit_message>
<xml_diff>
--- a/status reports/erica.xlsx
+++ b/status reports/erica.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -79,6 +79,14 @@
   </si>
   <si>
     <t>Research Implant Company</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1/24/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CFP Update/Edit</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -435,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -556,6 +564,17 @@
       </c>
       <c r="C10" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1.75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours update for erica
</commit_message>
<xml_diff>
--- a/status reports/erica.xlsx
+++ b/status reports/erica.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1"/>
@@ -131,6 +131,14 @@
   </si>
   <si>
     <t>CFP Update/Edit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2/6/2010</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CFP Update and misc</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -487,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -707,6 +715,17 @@
       </c>
       <c r="C19" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>